<commit_message>
Added Iteration 3 UI changes + Mode 2 Basic Game
</commit_message>
<xml_diff>
--- a/project documents/MathScramble_Project_WorkTrack_Report.xlsx
+++ b/project documents/MathScramble_Project_WorkTrack_Report.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
     <sheet name="Requirements" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 1" sheetId="3" r:id="rId3"/>
     <sheet name="Iteration 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Iteration 3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
   <si>
     <t>Seema Saijpaul</t>
   </si>
@@ -208,6 +209,33 @@
   </si>
   <si>
     <t>3. Completed the functionality to select equation on the screen</t>
+  </si>
+  <si>
+    <t>1.Implement changes to UI</t>
+  </si>
+  <si>
+    <t>2.Implement functionality of Puzzle (Basic + AI)</t>
+  </si>
+  <si>
+    <t>3.Implement enhancement of sound effect in equation game</t>
+  </si>
+  <si>
+    <t>4. Testing and Bug Fixing</t>
+  </si>
+  <si>
+    <t>5. Update code repository</t>
+  </si>
+  <si>
+    <t>1. Implemented changes to UI(Changed color scheme completely + Addition of animated button for bothe modes + sound effect on correct and wrong equation)</t>
+  </si>
+  <si>
+    <t>2. Implemented basic mode 2 game</t>
+  </si>
+  <si>
+    <t>3. Implemented AI functionality but still need to integrate with the system</t>
+  </si>
+  <si>
+    <t>4. Updated Code repository</t>
   </si>
 </sst>
 </file>
@@ -408,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -424,6 +452,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -855,55 +886,55 @@
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:14" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:14" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:14" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:14" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="21"/>
     </row>
     <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="J13" s="16"/>
-      <c r="K13" s="21" t="s">
+      <c r="J13" s="17"/>
+      <c r="K13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="24"/>
     </row>
     <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="J14" s="16"/>
-      <c r="K14" s="21" t="s">
+      <c r="J14" s="17"/>
+      <c r="K14" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="24"/>
     </row>
     <row r="15" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J15" s="17"/>
-      <c r="K15" s="24" t="s">
+      <c r="J15" s="18"/>
+      <c r="K15" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -935,13 +966,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1095,10 +1126,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="28"/>
+      <c r="B24" s="29"/>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
@@ -1106,10 +1137,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="28"/>
+      <c r="B26" s="29"/>
     </row>
     <row r="28" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -1150,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection sqref="A1:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,4 +1322,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>